<commit_message>
Analyse de la partie MenuPrincipale
</commit_message>
<xml_diff>
--- a/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
+++ b/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
-  <workbookPr showObjects="none" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr showObjects="none"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\ProjetPerso\TPIRTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TPI\ProjetUnity\TPI_CastleDefense\Assets\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05754AF-B9D5-4177-9A43-B9E46D7FF6FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30825" yWindow="-105" windowWidth="30930" windowHeight="16890"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -117,11 +116,57 @@
 Etablissement des sprints a faire
 Etablissement des tâches (dans les sprints)</t>
   </si>
+  <si>
+    <t>Envoie d'une proposition de mise en forme au chef de projet</t>
+  </si>
+  <si>
+    <t>Remise en forme
+du planning</t>
+  </si>
+  <si>
+    <t>Réception du rendez-vous de l'expert 2 demandant d'ajuster la planification en conséquence</t>
+  </si>
+  <si>
+    <t>Srprint Mise en Forme</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Remplissage de la partie Analyse préliminaire
+partie beaucoup plus longue et laborieuse qu'envisagée de par les terme a mettre dans le glossaire et les acronyme à mettre en bas de page</t>
+  </si>
+  <si>
+    <t>le week end sera LONG!</t>
+  </si>
+  <si>
+    <t>Analyse Menu Principale</t>
+  </si>
+  <si>
+    <t>Analyse prélinimaire</t>
+  </si>
+  <si>
+    <t>ötude de l'interface du jeu New World</t>
+  </si>
+  <si>
+    <t>Question sur l'organistion des sprint
+Convention de nommage
+Analyse et structure du Canvas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilisation de Icescrum
+Chaque élément du code doit être fixé
+Ne pas aller trop loin et ne mettre que des images ciblant précisément le sujet qui support l'illustration
+</t>
+  </si>
+  <si>
+    <t>Convention de Nommage</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -417,6 +462,26 @@
   </cellStyles>
   <dxfs count="12">
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="44"/>
+        </right>
+        <top style="thin">
+          <color indexed="44"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="44"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -441,26 +506,6 @@
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
-        <top style="thin">
-          <color indexed="44"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="44"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="44"/>
-        </right>
         <top style="thin">
           <color indexed="44"/>
         </top>
@@ -783,19 +828,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Journal" displayName="Journal" ref="A1:H81" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8">
-  <autoFilter ref="A1:H81" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Journal" displayName="Journal" ref="A1:H81" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8">
+  <autoFilter ref="A1:H81"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Début" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Fin" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Heure" dataDxfId="4">
+    <tableColumn id="1" name="Date" dataDxfId="7"/>
+    <tableColumn id="2" name="Début" dataDxfId="6"/>
+    <tableColumn id="3" name="Fin" dataDxfId="5"/>
+    <tableColumn id="4" name="Heure" dataDxfId="4">
       <calculatedColumnFormula>C2-B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Tâche" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Description" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Solutions" dataDxfId="0"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Sources" dataDxfId="1" dataCellStyle="Lien hypertexte"/>
+    <tableColumn id="5" name="Tâche" dataDxfId="3"/>
+    <tableColumn id="6" name="Description" dataDxfId="2"/>
+    <tableColumn id="7" name="Solutions" dataDxfId="1"/>
+    <tableColumn id="9" name="Sources" dataDxfId="0" dataCellStyle="Lien hypertexte"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1097,23 +1142,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" customWidth="1"/>
-    <col min="6" max="6" width="50.6640625" customWidth="1"/>
-    <col min="7" max="7" width="100.6640625" customWidth="1"/>
-    <col min="8" max="8" width="50.6640625" customWidth="1"/>
+    <col min="1" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" customWidth="1"/>
+    <col min="7" max="7" width="100.7109375" customWidth="1"/>
+    <col min="8" max="8" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1139,7 +1184,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>44683</v>
       </c>
@@ -1162,7 +1207,7 @@
       <c r="G2" s="6"/>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>44683</v>
       </c>
@@ -1185,7 +1230,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>44683</v>
       </c>
@@ -1208,7 +1253,7 @@
       <c r="G4" s="6"/>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>44683</v>
       </c>
@@ -1231,7 +1276,7 @@
       <c r="G5" s="6"/>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>44683</v>
       </c>
@@ -1256,85 +1301,147 @@
       </c>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+    <row r="7" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>44684</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.34513888888888888</v>
+      </c>
       <c r="D7" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="21"/>
+        <v>1.1805555555555569E-2</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>22</v>
+      </c>
       <c r="G7" s="6"/>
       <c r="H7" s="9"/>
     </row>
-    <row r="8" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+    <row r="8" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>44684</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.34513888888888888</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.35416666666666669</v>
+      </c>
       <c r="D8" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="21"/>
+        <v>9.0277777777778012E-3</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>24</v>
+      </c>
       <c r="G8" s="6"/>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+    <row r="9" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>44684</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.43263888888888885</v>
+      </c>
       <c r="D9" s="4">
         <f t="shared" ref="D9:D18" si="1">C9-B9</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="6"/>
+        <v>7.8472222222222165E-2</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
+    <row r="10" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>44684</v>
+      </c>
+      <c r="B10" s="13">
+        <v>0.43263888888888885</v>
+      </c>
+      <c r="C10" s="13">
+        <v>0.47916666666666669</v>
+      </c>
       <c r="D10" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="15"/>
+        <v>4.6527777777777835E-2</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>31</v>
+      </c>
       <c r="H10" s="16"/>
     </row>
-    <row r="11" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+    <row r="11" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>44684</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="D11" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="6"/>
+        <v>3.1249999999999944E-2</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="H11" s="9"/>
     </row>
-    <row r="12" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
+    <row r="12" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>44684</v>
+      </c>
+      <c r="B12" s="13">
+        <v>0.5625</v>
+      </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="14"/>
+        <v>-0.5625</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>34</v>
+      </c>
       <c r="F12" s="22"/>
       <c r="G12" s="15"/>
       <c r="H12" s="16"/>
     </row>
-    <row r="13" spans="1:8" ht="324.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="324.60000000000002" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1349,7 +1456,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -1362,7 +1469,7 @@
       <c r="G14" s="15"/>
       <c r="H14" s="16"/>
     </row>
-    <row r="15" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="27"/>
       <c r="B15" s="24"/>
       <c r="C15" s="24"/>
@@ -1375,7 +1482,7 @@
       <c r="G15" s="26"/>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27"/>
       <c r="B16" s="24"/>
       <c r="C16" s="24"/>
@@ -1388,7 +1495,7 @@
       <c r="G16" s="26"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="27"/>
       <c r="B17" s="24"/>
       <c r="C17" s="24"/>
@@ -1401,7 +1508,7 @@
       <c r="G17" s="26"/>
       <c r="H17" s="9"/>
     </row>
-    <row r="18" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="27"/>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
@@ -1414,7 +1521,7 @@
       <c r="G18" s="19"/>
       <c r="H18" s="20"/>
     </row>
-    <row r="19" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="27"/>
       <c r="B19" s="28"/>
       <c r="C19" s="28"/>
@@ -1427,7 +1534,7 @@
       <c r="G19" s="29"/>
       <c r="H19" s="20"/>
     </row>
-    <row r="20" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="27"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1440,7 +1547,7 @@
       <c r="G20" s="6"/>
       <c r="H20" s="9"/>
     </row>
-    <row r="21" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="27"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1453,7 +1560,7 @@
       <c r="G21" s="6"/>
       <c r="H21" s="9"/>
     </row>
-    <row r="22" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="27"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1466,7 +1573,7 @@
       <c r="G22" s="6"/>
       <c r="H22" s="9"/>
     </row>
-    <row r="23" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="27"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1479,7 +1586,7 @@
       <c r="G23" s="6"/>
       <c r="H23" s="9"/>
     </row>
-    <row r="24" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1492,7 +1599,7 @@
       <c r="G24" s="6"/>
       <c r="H24" s="9"/>
     </row>
-    <row r="25" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1505,7 +1612,7 @@
       <c r="G25" s="6"/>
       <c r="H25" s="9"/>
     </row>
-    <row r="26" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1518,7 +1625,7 @@
       <c r="G26" s="6"/>
       <c r="H26" s="9"/>
     </row>
-    <row r="27" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1531,7 +1638,7 @@
       <c r="G27" s="6"/>
       <c r="H27" s="9"/>
     </row>
-    <row r="28" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1544,7 +1651,7 @@
       <c r="G28" s="6"/>
       <c r="H28" s="9"/>
     </row>
-    <row r="29" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1557,7 +1664,7 @@
       <c r="G29" s="6"/>
       <c r="H29" s="9"/>
     </row>
-    <row r="30" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="31"/>
       <c r="B30" s="18"/>
       <c r="C30" s="18"/>
@@ -1570,7 +1677,7 @@
       <c r="G30" s="19"/>
       <c r="H30" s="20"/>
     </row>
-    <row r="31" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1583,7 +1690,7 @@
       <c r="G31" s="6"/>
       <c r="H31" s="9"/>
     </row>
-    <row r="32" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="31"/>
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
@@ -1596,7 +1703,7 @@
       <c r="G32" s="19"/>
       <c r="H32" s="20"/>
     </row>
-    <row r="33" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1609,7 +1716,7 @@
       <c r="G33" s="6"/>
       <c r="H33" s="9"/>
     </row>
-    <row r="34" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="31"/>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
@@ -1622,7 +1729,7 @@
       <c r="G34" s="19"/>
       <c r="H34" s="20"/>
     </row>
-    <row r="35" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1635,7 +1742,7 @@
       <c r="G35" s="6"/>
       <c r="H35" s="9"/>
     </row>
-    <row r="36" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1648,7 +1755,7 @@
       <c r="G36" s="6"/>
       <c r="H36" s="9"/>
     </row>
-    <row r="37" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="31"/>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
@@ -1661,7 +1768,7 @@
       <c r="G37" s="19"/>
       <c r="H37" s="20"/>
     </row>
-    <row r="38" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1674,7 +1781,7 @@
       <c r="G38" s="6"/>
       <c r="H38" s="9"/>
     </row>
-    <row r="39" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="31"/>
       <c r="B39" s="18"/>
       <c r="C39" s="18"/>
@@ -1687,7 +1794,7 @@
       <c r="G39" s="19"/>
       <c r="H39" s="20"/>
     </row>
-    <row r="40" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1700,7 +1807,7 @@
       <c r="G40" s="6"/>
       <c r="H40" s="9"/>
     </row>
-    <row r="41" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="31"/>
       <c r="B41" s="18"/>
       <c r="C41" s="18"/>
@@ -1713,7 +1820,7 @@
       <c r="G41" s="19"/>
       <c r="H41" s="20"/>
     </row>
-    <row r="42" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1726,7 +1833,7 @@
       <c r="G42" s="6"/>
       <c r="H42" s="9"/>
     </row>
-    <row r="43" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="31"/>
       <c r="B43" s="18"/>
       <c r="C43" s="18"/>
@@ -1739,7 +1846,7 @@
       <c r="G43" s="19"/>
       <c r="H43" s="20"/>
     </row>
-    <row r="44" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -1752,7 +1859,7 @@
       <c r="G44" s="6"/>
       <c r="H44" s="9"/>
     </row>
-    <row r="45" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="31"/>
       <c r="B45" s="18"/>
       <c r="C45" s="18"/>
@@ -1765,7 +1872,7 @@
       <c r="G45" s="19"/>
       <c r="H45" s="20"/>
     </row>
-    <row r="46" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -1778,7 +1885,7 @@
       <c r="G46" s="6"/>
       <c r="H46" s="9"/>
     </row>
-    <row r="47" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="31"/>
       <c r="B47" s="18"/>
       <c r="C47" s="18"/>
@@ -1791,7 +1898,7 @@
       <c r="G47" s="19"/>
       <c r="H47" s="20"/>
     </row>
-    <row r="48" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -1804,7 +1911,7 @@
       <c r="G48" s="6"/>
       <c r="H48" s="9"/>
     </row>
-    <row r="49" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="31"/>
       <c r="B49" s="18"/>
       <c r="C49" s="18"/>
@@ -1817,7 +1924,7 @@
       <c r="G49" s="19"/>
       <c r="H49" s="20"/>
     </row>
-    <row r="50" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -1830,7 +1937,7 @@
       <c r="G50" s="6"/>
       <c r="H50" s="9"/>
     </row>
-    <row r="51" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="31"/>
       <c r="B51" s="18"/>
       <c r="C51" s="18"/>
@@ -1843,7 +1950,7 @@
       <c r="G51" s="19"/>
       <c r="H51" s="20"/>
     </row>
-    <row r="52" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -1856,7 +1963,7 @@
       <c r="G52" s="6"/>
       <c r="H52" s="9"/>
     </row>
-    <row r="53" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="31"/>
       <c r="B53" s="18"/>
       <c r="C53" s="18"/>
@@ -1869,7 +1976,7 @@
       <c r="G53" s="19"/>
       <c r="H53" s="20"/>
     </row>
-    <row r="54" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -1882,7 +1989,7 @@
       <c r="G54" s="6"/>
       <c r="H54" s="9"/>
     </row>
-    <row r="55" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="31"/>
       <c r="B55" s="18"/>
       <c r="C55" s="18"/>
@@ -1895,7 +2002,7 @@
       <c r="G55" s="19"/>
       <c r="H55" s="20"/>
     </row>
-    <row r="56" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -1908,7 +2015,7 @@
       <c r="G56" s="6"/>
       <c r="H56" s="9"/>
     </row>
-    <row r="57" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="31"/>
       <c r="B57" s="18"/>
       <c r="C57" s="18"/>
@@ -1921,7 +2028,7 @@
       <c r="G57" s="19"/>
       <c r="H57" s="20"/>
     </row>
-    <row r="58" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -1934,7 +2041,7 @@
       <c r="G58" s="6"/>
       <c r="H58" s="9"/>
     </row>
-    <row r="59" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="31"/>
       <c r="B59" s="18"/>
       <c r="C59" s="18"/>
@@ -1947,7 +2054,7 @@
       <c r="G59" s="19"/>
       <c r="H59" s="20"/>
     </row>
-    <row r="60" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -1960,7 +2067,7 @@
       <c r="G60" s="6"/>
       <c r="H60" s="9"/>
     </row>
-    <row r="61" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="31"/>
       <c r="B61" s="18"/>
       <c r="C61" s="18"/>
@@ -1973,7 +2080,7 @@
       <c r="G61" s="19"/>
       <c r="H61" s="20"/>
     </row>
-    <row r="62" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -1986,7 +2093,7 @@
       <c r="G62" s="6"/>
       <c r="H62" s="9"/>
     </row>
-    <row r="63" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="31"/>
       <c r="B63" s="18"/>
       <c r="C63" s="18"/>
@@ -1999,7 +2106,7 @@
       <c r="G63" s="19"/>
       <c r="H63" s="20"/>
     </row>
-    <row r="64" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -2012,7 +2119,7 @@
       <c r="G64" s="6"/>
       <c r="H64" s="9"/>
     </row>
-    <row r="65" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="31"/>
       <c r="B65" s="18"/>
       <c r="C65" s="18"/>
@@ -2025,7 +2132,7 @@
       <c r="G65" s="19"/>
       <c r="H65" s="20"/>
     </row>
-    <row r="66" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -2038,7 +2145,7 @@
       <c r="G66" s="6"/>
       <c r="H66" s="9"/>
     </row>
-    <row r="67" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="31"/>
       <c r="B67" s="18"/>
       <c r="C67" s="18"/>
@@ -2051,7 +2158,7 @@
       <c r="G67" s="19"/>
       <c r="H67" s="20"/>
     </row>
-    <row r="68" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -2064,7 +2171,7 @@
       <c r="G68" s="6"/>
       <c r="H68" s="9"/>
     </row>
-    <row r="69" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="31"/>
       <c r="B69" s="18"/>
       <c r="C69" s="18"/>
@@ -2077,7 +2184,7 @@
       <c r="G69" s="19"/>
       <c r="H69" s="20"/>
     </row>
-    <row r="70" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -2090,7 +2197,7 @@
       <c r="G70" s="6"/>
       <c r="H70" s="9"/>
     </row>
-    <row r="71" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="31"/>
       <c r="B71" s="18"/>
       <c r="C71" s="18"/>
@@ -2103,7 +2210,7 @@
       <c r="G71" s="19"/>
       <c r="H71" s="20"/>
     </row>
-    <row r="72" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -2116,7 +2223,7 @@
       <c r="G72" s="6"/>
       <c r="H72" s="9"/>
     </row>
-    <row r="73" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="31"/>
       <c r="B73" s="18"/>
       <c r="C73" s="18"/>
@@ -2129,7 +2236,7 @@
       <c r="G73" s="19"/>
       <c r="H73" s="20"/>
     </row>
-    <row r="74" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -2142,7 +2249,7 @@
       <c r="G74" s="6"/>
       <c r="H74" s="9"/>
     </row>
-    <row r="75" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="31"/>
       <c r="B75" s="18"/>
       <c r="C75" s="18"/>
@@ -2155,7 +2262,7 @@
       <c r="G75" s="19"/>
       <c r="H75" s="20"/>
     </row>
-    <row r="76" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -2168,7 +2275,7 @@
       <c r="G76" s="6"/>
       <c r="H76" s="9"/>
     </row>
-    <row r="77" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="31"/>
       <c r="B77" s="18"/>
       <c r="C77" s="18"/>
@@ -2181,7 +2288,7 @@
       <c r="G77" s="19"/>
       <c r="H77" s="20"/>
     </row>
-    <row r="78" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -2194,7 +2301,7 @@
       <c r="G78" s="6"/>
       <c r="H78" s="9"/>
     </row>
-    <row r="79" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="31"/>
       <c r="B79" s="18"/>
       <c r="C79" s="18"/>
@@ -2207,7 +2314,7 @@
       <c r="G79" s="19"/>
       <c r="H79" s="20"/>
     </row>
-    <row r="80" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>44659</v>
       </c>
@@ -2230,7 +2337,7 @@
       <c r="G80" s="6"/>
       <c r="H80" s="9"/>
     </row>
-    <row r="81" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="31">
         <v>44660</v>
       </c>

</xml_diff>

<commit_message>
Ajout de la documentation concernant Les tests d'acceptation
- Menu principal
- Interaction régiment
</commit_message>
<xml_diff>
--- a/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
+++ b/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>Date</t>
   </si>
@@ -174,6 +174,38 @@
   </si>
   <si>
     <t>migration des sprint de github à icescrum</t>
+  </si>
+  <si>
+    <t>Sprint semain1</t>
+  </si>
+  <si>
+    <t>Sprint Semaine 2</t>
+  </si>
+  <si>
+    <t>Use Case</t>
+  </si>
+  <si>
+    <t>Regiment et Unité: définition des concernes</t>
+  </si>
+  <si>
+    <t>Implémentation du Menu</t>
+  </si>
+  <si>
+    <t>Implémentattion des la partie graphique selon maquette</t>
+  </si>
+  <si>
+    <t>Menu : Fonction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implémentation des fonctions liées au menu </t>
+  </si>
+  <si>
+    <t>Documentation de
+la partie Tests de validation</t>
+  </si>
+  <si>
+    <t>Menu principale
+Intéraction régiment</t>
   </si>
 </sst>
 </file>
@@ -1155,8 +1187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,51 +1536,85 @@
       <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
+      <c r="A15" s="26">
+        <v>44685</v>
+      </c>
+      <c r="B15" s="23">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="C15" s="23">
+        <v>0.39583333333333331</v>
+      </c>
       <c r="D15" s="23">
         <f>C15-B15</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="24"/>
+        <v>2.7777777777777735E-2</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>40</v>
+      </c>
       <c r="G15" s="25"/>
       <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
+      <c r="A16" s="26">
+        <v>44685</v>
+      </c>
+      <c r="B16" s="23">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="C16" s="23">
+        <v>0.4381944444444445</v>
+      </c>
       <c r="D16" s="23">
         <f>C16-B16</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="13"/>
+        <v>2.8472222222222232E-2</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>41</v>
+      </c>
       <c r="F16" s="24"/>
       <c r="G16" s="25"/>
       <c r="H16" s="9"/>
     </row>
     <row r="17" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
+      <c r="A17" s="26">
+        <v>44685</v>
+      </c>
+      <c r="B17" s="23">
+        <v>0.4381944444444445</v>
+      </c>
+      <c r="C17" s="23">
+        <v>0.46388888888888885</v>
+      </c>
       <c r="D17" s="23">
         <f>C17-B17</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="24"/>
+        <v>2.5694444444444353E-2</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>43</v>
+      </c>
       <c r="G17" s="25"/>
       <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
+      <c r="A18" s="26">
+        <v>44685</v>
+      </c>
+      <c r="B18" s="17">
+        <v>0.46388888888888885</v>
+      </c>
+      <c r="C18" s="17">
+        <v>0.49027777777777781</v>
+      </c>
       <c r="D18" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.6388888888888962E-2</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="22"/>
@@ -1556,53 +1622,91 @@
       <c r="H18" s="19"/>
     </row>
     <row r="19" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
+      <c r="A19" s="26">
+        <v>44685</v>
+      </c>
+      <c r="B19" s="27">
+        <v>0.49027777777777781</v>
+      </c>
+      <c r="C19" s="27">
+        <v>0.50347222222222221</v>
+      </c>
       <c r="D19" s="27">
         <f>C19-B19</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="22"/>
+        <v>1.3194444444444398E-2</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G19" s="28"/>
       <c r="H19" s="19"/>
     </row>
     <row r="20" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
+      <c r="A20" s="26">
+        <v>44685</v>
+      </c>
+      <c r="B20" s="4">
+        <v>0.56180555555555556</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.57777777777777783</v>
+      </c>
       <c r="D20" s="4">
         <f t="shared" ref="D20" si="2">C20-B20</f>
-        <v>0</v>
-      </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="20"/>
+        <v>1.5972222222222276E-2</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>47</v>
+      </c>
       <c r="G20" s="6"/>
       <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
+      <c r="A21" s="26">
+        <v>44685</v>
+      </c>
+      <c r="B21" s="4">
+        <v>0.57777777777777783</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.61736111111111114</v>
+      </c>
       <c r="D21" s="4">
         <f>C21-B21</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="20"/>
+        <v>3.9583333333333304E-2</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>49</v>
+      </c>
       <c r="G21" s="6"/>
       <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
+      <c r="A22" s="26">
+        <v>44685</v>
+      </c>
+      <c r="B22" s="4">
+        <v>0.61736111111111114</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.65763888888888888</v>
+      </c>
       <c r="D22" s="4">
         <f t="shared" ref="D22" si="3">C22-B22</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="13"/>
+        <v>4.0277777777777746E-2</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>25</v>
+      </c>
       <c r="F22" s="20"/>
       <c r="G22" s="6"/>
       <c r="H22" s="9"/>

</xml_diff>

<commit_message>
Prototypage du système d'interface des registres lié à ll'intéractions avec les régiments
</commit_message>
<xml_diff>
--- a/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
+++ b/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="78">
   <si>
     <t>Date</t>
   </si>
@@ -264,6 +264,39 @@
   </si>
   <si>
     <t>Documentation sur le choix de la structure des régiment selon directive</t>
+  </si>
+  <si>
+    <t>Analyse des besoins pour le système régiment</t>
+  </si>
+  <si>
+    <t>Définition des besoins en terme de comportements
+comportement similaires entre les composantes
+potentiel candidat pour les interfaces ou abtracts</t>
+  </si>
+  <si>
+    <t>Prototypage rudimentaire sur base de l'analyse</t>
+  </si>
+  <si>
+    <t>Préparation de base de l'environnement Unity</t>
+  </si>
+  <si>
+    <t>Preparation des prefabs notamment les factory précréer afin de faciliter le prototypage</t>
+  </si>
+  <si>
+    <t>Gros Soucis de conception, il faut reprendre depuis le début et bien cerner les responsabilité de chaque classe</t>
+  </si>
+  <si>
+    <t>Suite Prototypage</t>
+  </si>
+  <si>
+    <t>redéfinition des interface selon les observation précédentes</t>
+  </si>
+  <si>
+    <t>L'implémentation a pris plus de temps, car il a fallu adapter plus d'élément que prévu
+Cependant l'architecture smelbe être solide en l'état</t>
+  </si>
+  <si>
+    <t>Soucis liées aux interface sur Unity</t>
   </si>
 </sst>
 </file>
@@ -1248,8 +1281,8 @@
   </sheetPr>
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2077,66 +2110,116 @@
       <c r="H36" s="9"/>
     </row>
     <row r="37" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="17"/>
+      <c r="A37" s="30">
+        <v>44691</v>
+      </c>
+      <c r="B37" s="17">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C37" s="17">
+        <v>0.40347222222222223</v>
+      </c>
       <c r="D37" s="17">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E37" s="29"/>
-      <c r="F37" s="22"/>
+        <v>7.0138888888888917E-2</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="F37" s="22" t="s">
+        <v>69</v>
+      </c>
       <c r="G37" s="18"/>
       <c r="H37" s="19"/>
     </row>
     <row r="38" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
+      <c r="A38" s="3">
+        <v>44691</v>
+      </c>
+      <c r="B38" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0.4375</v>
+      </c>
       <c r="D38" s="4">
         <f t="shared" ref="D38:D41" si="6">C38-B38</f>
-        <v>0</v>
-      </c>
-      <c r="E38" s="29"/>
-      <c r="F38" s="20"/>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="E38" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="F38" s="20" t="s">
+        <v>72</v>
+      </c>
       <c r="G38" s="6"/>
       <c r="H38" s="9"/>
     </row>
     <row r="39" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
+      <c r="A39" s="30">
+        <v>44691</v>
+      </c>
+      <c r="B39" s="17">
+        <v>0.4375</v>
+      </c>
+      <c r="C39" s="17">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="D39" s="17">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E39" s="29"/>
-      <c r="F39" s="22"/>
+        <v>7.291666666666663E-2</v>
+      </c>
+      <c r="E39" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="F39" s="22" t="s">
+        <v>73</v>
+      </c>
       <c r="G39" s="18"/>
       <c r="H39" s="19"/>
     </row>
     <row r="40" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
+      <c r="A40" s="3">
+        <v>44691</v>
+      </c>
+      <c r="B40" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0.64444444444444449</v>
+      </c>
       <c r="D40" s="4">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E40" s="29"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="6"/>
+        <v>8.1944444444444486E-2</v>
+      </c>
+      <c r="E40" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="30"/>
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
+      <c r="A41" s="30">
+        <v>44691</v>
+      </c>
+      <c r="B41" s="17">
+        <v>0.64444444444444449</v>
+      </c>
+      <c r="C41" s="17">
+        <v>0.66319444444444442</v>
+      </c>
       <c r="D41" s="17">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E41" s="29"/>
+        <v>1.8749999999999933E-2</v>
+      </c>
+      <c r="E41" s="29" t="s">
+        <v>77</v>
+      </c>
       <c r="F41" s="22"/>
       <c r="G41" s="18"/>
       <c r="H41" s="19"/>

</xml_diff>

<commit_message>
Système de préselection Fonctionnelle
</commit_message>
<xml_diff>
--- a/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
+++ b/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="82">
   <si>
     <t>Date</t>
   </si>
@@ -297,6 +297,19 @@
   </si>
   <si>
     <t>Soucis liées aux interface sur Unity</t>
+  </si>
+  <si>
+    <t>Relecture de la documentation</t>
+  </si>
+  <si>
+    <t>vérification de l'orhographe et de la grammaire
+réimportation d'images qui étaient de mauvaises qualitées</t>
+  </si>
+  <si>
+    <t>System de Preselection fonctionnelle</t>
+  </si>
+  <si>
+    <t>Documentation Selon Model</t>
   </si>
 </sst>
 </file>
@@ -1281,8 +1294,8 @@
   </sheetPr>
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2225,40 +2238,64 @@
       <c r="H41" s="19"/>
     </row>
     <row r="42" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
+      <c r="A42" s="3">
+        <v>44692</v>
+      </c>
+      <c r="B42" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C42" s="4">
+        <v>0.36805555555555558</v>
+      </c>
       <c r="D42" s="4">
         <f t="shared" ref="D42:D81" si="7">C42-B42</f>
-        <v>0</v>
-      </c>
-      <c r="E42" s="29"/>
-      <c r="F42" s="20"/>
+        <v>3.4722222222222265E-2</v>
+      </c>
+      <c r="E42" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="F42" s="20" t="s">
+        <v>79</v>
+      </c>
       <c r="G42" s="6"/>
       <c r="H42" s="9"/>
     </row>
     <row r="43" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="30"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="17"/>
+      <c r="A43" s="30">
+        <v>44692</v>
+      </c>
+      <c r="B43" s="17">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="C43" s="17">
+        <v>0.45</v>
+      </c>
       <c r="D43" s="17">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E43" s="29"/>
+        <v>8.1944444444444431E-2</v>
+      </c>
+      <c r="E43" s="29" t="s">
+        <v>80</v>
+      </c>
       <c r="F43" s="22"/>
       <c r="G43" s="18"/>
       <c r="H43" s="19"/>
     </row>
     <row r="44" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="4"/>
+      <c r="A44" s="3">
+        <v>44692</v>
+      </c>
+      <c r="B44" s="4">
+        <v>0.45</v>
+      </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E44" s="29"/>
+        <v>-0.45</v>
+      </c>
+      <c r="E44" s="29" t="s">
+        <v>81</v>
+      </c>
       <c r="F44" s="20"/>
       <c r="G44" s="6"/>
       <c r="H44" s="9"/>

</xml_diff>

<commit_message>
Correction de la preselection + Documentation sur la preselection(introduction, enjeux, diagramme)
</commit_message>
<xml_diff>
--- a/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
+++ b/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="89">
   <si>
     <t>Date</t>
   </si>
@@ -309,7 +309,31 @@
     <t>System de Preselection fonctionnelle</t>
   </si>
   <si>
-    <t>Documentation Selon Model</t>
+    <t>Lecture sur les convensions d'écritures UML</t>
+  </si>
+  <si>
+    <t>https://www.uml-diagrams.org/abstraction.html</t>
+  </si>
+  <si>
+    <t>Lecture sur la convention concernant les abstract et les interfaces et leur représentation dans un schéma</t>
+  </si>
+  <si>
+    <t>Diagramme de classe
+Régiment</t>
+  </si>
+  <si>
+    <t>BUG avec certains régiments</t>
+  </si>
+  <si>
+    <t>L'interface Repassait dans tout le registre, ce qui réinitialisait les valeur des autres régiments, précédemment enregistré</t>
+  </si>
+  <si>
+    <t>Documentation:
+Preselection
+Diagram de flux</t>
+  </si>
+  <si>
+    <t>Documentation Selection</t>
   </si>
 </sst>
 </file>
@@ -1294,8 +1318,8 @@
   </sheetPr>
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2288,66 +2312,106 @@
       <c r="B44" s="4">
         <v>0.45</v>
       </c>
-      <c r="C44" s="4"/>
+      <c r="C44" s="4">
+        <v>0.48194444444444445</v>
+      </c>
       <c r="D44" s="4">
         <f t="shared" si="7"/>
-        <v>-0.45</v>
+        <v>3.1944444444444442E-2</v>
       </c>
       <c r="E44" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="F44" s="20"/>
+      <c r="F44" s="20" t="s">
+        <v>83</v>
+      </c>
       <c r="G44" s="6"/>
-      <c r="H44" s="9"/>
+      <c r="H44" s="9" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="45" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="30"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="17"/>
+      <c r="A45" s="30">
+        <v>44692</v>
+      </c>
+      <c r="B45" s="17">
+        <v>0.48194444444444445</v>
+      </c>
+      <c r="C45" s="17">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="D45" s="17">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E45" s="29"/>
+        <v>2.8472222222222177E-2</v>
+      </c>
+      <c r="E45" s="29" t="s">
+        <v>84</v>
+      </c>
       <c r="F45" s="22"/>
       <c r="G45" s="18"/>
       <c r="H45" s="19"/>
     </row>
     <row r="46" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
+      <c r="A46" s="3">
+        <v>44692</v>
+      </c>
+      <c r="B46" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0.56944444444444442</v>
+      </c>
       <c r="D46" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E46" s="29"/>
-      <c r="F46" s="20"/>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="E46" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="F46" s="20" t="s">
+        <v>86</v>
+      </c>
       <c r="G46" s="6"/>
       <c r="H46" s="9"/>
     </row>
     <row r="47" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="30"/>
-      <c r="B47" s="17"/>
-      <c r="C47" s="17"/>
+      <c r="A47" s="30">
+        <v>44692</v>
+      </c>
+      <c r="B47" s="17">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="C47" s="17">
+        <v>0.6333333333333333</v>
+      </c>
       <c r="D47" s="17">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E47" s="29"/>
+        <v>6.3888888888888884E-2</v>
+      </c>
+      <c r="E47" s="29" t="s">
+        <v>87</v>
+      </c>
       <c r="F47" s="22"/>
       <c r="G47" s="18"/>
       <c r="H47" s="19"/>
     </row>
     <row r="48" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
+      <c r="A48" s="3">
+        <v>44692</v>
+      </c>
+      <c r="B48" s="4">
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="C48" s="4">
+        <v>0.70486111111111116</v>
+      </c>
       <c r="D48" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E48" s="29"/>
+        <v>7.1527777777777857E-2</v>
+      </c>
+      <c r="E48" s="29" t="s">
+        <v>88</v>
+      </c>
       <c r="F48" s="20"/>
       <c r="G48" s="6"/>
       <c r="H48" s="9"/>
@@ -2802,11 +2866,14 @@
       <c r="H81" s="19"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H44" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="12" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="12" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Conception du placement des unités et algorithme associé
</commit_message>
<xml_diff>
--- a/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
+++ b/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
   <si>
     <t>Date</t>
   </si>
@@ -334,6 +334,15 @@
   </si>
   <si>
     <t>Documentation Selection</t>
+  </si>
+  <si>
+    <t>Documentation Selection + UML</t>
+  </si>
+  <si>
+    <t>Analyse de la partie Placement</t>
+  </si>
+  <si>
+    <t>Explication de chaque phase du placement + algorithme</t>
   </si>
 </sst>
 </file>
@@ -1318,8 +1327,8 @@
   </sheetPr>
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2417,40 +2426,62 @@
       <c r="H48" s="9"/>
     </row>
     <row r="49" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="30"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="17"/>
+      <c r="A49" s="30">
+        <v>44693</v>
+      </c>
+      <c r="B49" s="17">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C49" s="17">
+        <v>0.39930555555555558</v>
+      </c>
       <c r="D49" s="17">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E49" s="29"/>
+        <v>6.5972222222222265E-2</v>
+      </c>
+      <c r="E49" s="29" t="s">
+        <v>89</v>
+      </c>
       <c r="F49" s="22"/>
       <c r="G49" s="18"/>
       <c r="H49" s="19"/>
     </row>
     <row r="50" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
+      <c r="A50" s="3">
+        <v>44693</v>
+      </c>
+      <c r="B50" s="4">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="C50" s="4">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="D50" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E50" s="29"/>
+        <v>0.10069444444444436</v>
+      </c>
+      <c r="E50" s="29" t="s">
+        <v>90</v>
+      </c>
       <c r="F50" s="20"/>
       <c r="G50" s="6"/>
       <c r="H50" s="9"/>
     </row>
     <row r="51" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="30"/>
-      <c r="B51" s="17"/>
+      <c r="A51" s="30">
+        <v>44693</v>
+      </c>
+      <c r="B51" s="17">
+        <v>0.5625</v>
+      </c>
       <c r="C51" s="17"/>
       <c r="D51" s="17">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E51" s="29"/>
+        <v>-0.5625</v>
+      </c>
+      <c r="E51" s="29" t="s">
+        <v>91</v>
+      </c>
       <c r="F51" s="22"/>
       <c r="G51" s="18"/>
       <c r="H51" s="19"/>

</xml_diff>

<commit_message>
Documentation sur l'algorithme placement/arrangement d'un régiment
</commit_message>
<xml_diff>
--- a/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
+++ b/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="93">
   <si>
     <t>Date</t>
   </si>
@@ -343,6 +343,9 @@
   </si>
   <si>
     <t>Explication de chaque phase du placement + algorithme</t>
+  </si>
+  <si>
+    <t>Expliquer un algorithme est plus long qu'imaginé, des sacrifice vont devoir être fait</t>
   </si>
 </sst>
 </file>
@@ -1327,8 +1330,8 @@
   </sheetPr>
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection sqref="A1:H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2474,15 +2477,19 @@
       <c r="B51" s="17">
         <v>0.5625</v>
       </c>
-      <c r="C51" s="17"/>
+      <c r="C51" s="17">
+        <v>0.70486111111111116</v>
+      </c>
       <c r="D51" s="17">
         <f t="shared" si="7"/>
-        <v>-0.5625</v>
+        <v>0.14236111111111116</v>
       </c>
       <c r="E51" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="F51" s="22"/>
+      <c r="F51" s="22" t="s">
+        <v>92</v>
+      </c>
       <c r="G51" s="18"/>
       <c r="H51" s="19"/>
     </row>
@@ -2901,7 +2908,7 @@
     <hyperlink ref="H44" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="12" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="33" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>

</xml_diff>

<commit_message>
Documentation concernant le placement multiple
- nouvelles contraintes
- taille différente + calcul
</commit_message>
<xml_diff>
--- a/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
+++ b/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="95">
   <si>
     <t>Date</t>
   </si>
@@ -346,6 +346,13 @@
   </si>
   <si>
     <t>Expliquer un algorithme est plus long qu'imaginé, des sacrifice vont devoir être fait</t>
+  </si>
+  <si>
+    <t>Fin de la doc concernant 
+le placement de 1 régiment</t>
+  </si>
+  <si>
+    <t>Algorithme avec plusieurs régiment(Placement)</t>
   </si>
 </sst>
 </file>
@@ -1330,8 +1337,8 @@
   </sheetPr>
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection sqref="A1:H51"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2494,27 +2501,43 @@
       <c r="H51" s="19"/>
     </row>
     <row r="52" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
+      <c r="A52" s="3">
+        <v>44697</v>
+      </c>
+      <c r="B52" s="4">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="C52" s="4">
+        <v>0.4375</v>
+      </c>
       <c r="D52" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E52" s="29"/>
+        <v>2.7777777777777735E-2</v>
+      </c>
+      <c r="E52" s="29" t="s">
+        <v>93</v>
+      </c>
       <c r="F52" s="20"/>
       <c r="G52" s="6"/>
       <c r="H52" s="9"/>
     </row>
     <row r="53" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="30"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="17"/>
+      <c r="A53" s="30">
+        <v>44697</v>
+      </c>
+      <c r="B53" s="17">
+        <v>0.4375</v>
+      </c>
+      <c r="C53" s="17">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="D53" s="17">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E53" s="29"/>
+        <v>7.291666666666663E-2</v>
+      </c>
+      <c r="E53" s="29" t="s">
+        <v>94</v>
+      </c>
       <c r="F53" s="22"/>
       <c r="G53" s="18"/>
       <c r="H53" s="19"/>

</xml_diff>

<commit_message>
Placement Multiple: Documentation et implémentations
</commit_message>
<xml_diff>
--- a/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
+++ b/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="97">
   <si>
     <t>Date</t>
   </si>
@@ -353,6 +353,12 @@
   </si>
   <si>
     <t>Algorithme avec plusieurs régiment(Placement)</t>
+  </si>
+  <si>
+    <t>Entretien avec chef de projet</t>
+  </si>
+  <si>
+    <t>Implémentation Placement multiple</t>
   </si>
 </sst>
 </file>
@@ -1337,8 +1343,8 @@
   </sheetPr>
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2543,27 +2549,43 @@
       <c r="H53" s="19"/>
     </row>
     <row r="54" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
+      <c r="A54" s="3">
+        <v>44697</v>
+      </c>
+      <c r="B54" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C54" s="4">
+        <v>0.60416666666666663</v>
+      </c>
       <c r="D54" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E54" s="29"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E54" s="29" t="s">
+        <v>96</v>
+      </c>
       <c r="F54" s="20"/>
       <c r="G54" s="6"/>
       <c r="H54" s="9"/>
     </row>
     <row r="55" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="30"/>
-      <c r="B55" s="17"/>
-      <c r="C55" s="17"/>
+      <c r="A55" s="30">
+        <v>44697</v>
+      </c>
+      <c r="B55" s="17">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C55" s="17">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="D55" s="17">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E55" s="29"/>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="E55" s="29" t="s">
+        <v>95</v>
+      </c>
       <c r="F55" s="22"/>
       <c r="G55" s="18"/>
       <c r="H55" s="19"/>

</xml_diff>

<commit_message>
Documentation HPA Introduction et analyse
</commit_message>
<xml_diff>
--- a/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
+++ b/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="99">
   <si>
     <t>Date</t>
   </si>
@@ -359,6 +359,12 @@
   </si>
   <si>
     <t>Implémentation Placement multiple</t>
+  </si>
+  <si>
+    <t>Analyse HPA</t>
+  </si>
+  <si>
+    <t>Introduction et présentation du HPA</t>
   </si>
 </sst>
 </file>
@@ -1343,8 +1349,8 @@
   </sheetPr>
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2591,27 +2597,43 @@
       <c r="H55" s="19"/>
     </row>
     <row r="56" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="3"/>
-      <c r="B56" s="4"/>
-      <c r="C56" s="4"/>
+      <c r="A56" s="3">
+        <v>44698</v>
+      </c>
+      <c r="B56" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C56" s="4">
+        <v>0.39583333333333331</v>
+      </c>
       <c r="D56" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E56" s="29"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E56" s="29" t="s">
+        <v>97</v>
+      </c>
       <c r="F56" s="20"/>
       <c r="G56" s="6"/>
       <c r="H56" s="9"/>
     </row>
     <row r="57" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="30"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
+      <c r="A57" s="30">
+        <v>44698</v>
+      </c>
+      <c r="B57" s="17">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C57" s="17">
+        <v>0.43541666666666662</v>
+      </c>
       <c r="D57" s="17">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E57" s="29"/>
+        <v>3.9583333333333304E-2</v>
+      </c>
+      <c r="E57" s="29" t="s">
+        <v>98</v>
+      </c>
       <c r="F57" s="22"/>
       <c r="G57" s="18"/>
       <c r="H57" s="19"/>

</xml_diff>

<commit_message>
Mise a jour des documents administratifs
</commit_message>
<xml_diff>
--- a/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
+++ b/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="102">
   <si>
     <t>Date</t>
   </si>
@@ -365,6 +365,15 @@
   </si>
   <si>
     <t>Introduction et présentation du HPA</t>
+  </si>
+  <si>
+    <t>documentation</t>
+  </si>
+  <si>
+    <t>HPA: Conception</t>
+  </si>
+  <si>
+    <t>Entretien avec le second expert</t>
   </si>
 </sst>
 </file>
@@ -1349,8 +1358,8 @@
   </sheetPr>
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2639,53 +2648,85 @@
       <c r="H57" s="19"/>
     </row>
     <row r="58" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="3"/>
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
+      <c r="A58" s="3">
+        <v>44698</v>
+      </c>
+      <c r="B58" s="4">
+        <v>0.43541666666666662</v>
+      </c>
+      <c r="C58" s="4">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="D58" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E58" s="29"/>
+        <v>7.5000000000000011E-2</v>
+      </c>
+      <c r="E58" s="29" t="s">
+        <v>99</v>
+      </c>
       <c r="F58" s="20"/>
       <c r="G58" s="6"/>
       <c r="H58" s="9"/>
     </row>
     <row r="59" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="30"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="17"/>
+      <c r="A59" s="30">
+        <v>44698</v>
+      </c>
+      <c r="B59" s="17">
+        <v>0.5625</v>
+      </c>
+      <c r="C59" s="17">
+        <v>0.61805555555555558</v>
+      </c>
       <c r="D59" s="17">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E59" s="29"/>
+        <v>5.555555555555558E-2</v>
+      </c>
+      <c r="E59" s="29" t="s">
+        <v>100</v>
+      </c>
       <c r="F59" s="22"/>
       <c r="G59" s="18"/>
       <c r="H59" s="19"/>
     </row>
     <row r="60" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="3"/>
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
+      <c r="A60" s="3">
+        <v>44698</v>
+      </c>
+      <c r="B60" s="4">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="C60" s="4">
+        <v>0.64583333333333337</v>
+      </c>
       <c r="D60" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E60" s="29"/>
+        <v>2.777777777777779E-2</v>
+      </c>
+      <c r="E60" s="29" t="s">
+        <v>100</v>
+      </c>
       <c r="F60" s="20"/>
       <c r="G60" s="6"/>
       <c r="H60" s="9"/>
     </row>
     <row r="61" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="30"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="17"/>
+      <c r="A61" s="30">
+        <v>44698</v>
+      </c>
+      <c r="B61" s="17">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C61" s="17">
+        <v>0.67013888888888884</v>
+      </c>
       <c r="D61" s="17">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E61" s="29"/>
+        <v>2.4305555555555469E-2</v>
+      </c>
+      <c r="E61" s="29" t="s">
+        <v>101</v>
+      </c>
       <c r="F61" s="22"/>
       <c r="G61" s="18"/>
       <c r="H61" s="19"/>

</xml_diff>

<commit_message>
Mise a jour de la documentation: HPA
</commit_message>
<xml_diff>
--- a/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
+++ b/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="108">
   <si>
     <t>Date</t>
   </si>
@@ -374,6 +374,26 @@
   </si>
   <si>
     <t>Entretien avec le second expert</t>
+  </si>
+  <si>
+    <t>Prototypage rudimentaire pour vérifier la compatibilité de certain container</t>
+  </si>
+  <si>
+    <t>Il y a un risque lié à la limitation des container Natif utilisé par Unity pour le jobSystem</t>
+  </si>
+  <si>
+    <t>Prototypage: trouver les portes de chaque chunk</t>
+  </si>
+  <si>
+    <t>Documentation HPA</t>
+  </si>
+  <si>
+    <t>début
+Grille
+Structure de données des portes</t>
+  </si>
+  <si>
+    <t>Documentation Datastructure/Architecture du programme</t>
   </si>
 </sst>
 </file>
@@ -1358,8 +1378,8 @@
   </sheetPr>
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2732,53 +2752,89 @@
       <c r="H61" s="19"/>
     </row>
     <row r="62" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="3"/>
-      <c r="B62" s="4"/>
-      <c r="C62" s="4"/>
+      <c r="A62" s="3">
+        <v>44699</v>
+      </c>
+      <c r="B62" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C62" s="4">
+        <v>0.4375</v>
+      </c>
       <c r="D62" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E62" s="29"/>
-      <c r="F62" s="20"/>
+        <v>0.10416666666666669</v>
+      </c>
+      <c r="E62" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="F62" s="20" t="s">
+        <v>103</v>
+      </c>
       <c r="G62" s="6"/>
       <c r="H62" s="9"/>
     </row>
     <row r="63" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="30"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="17"/>
+      <c r="A63" s="30">
+        <v>44699</v>
+      </c>
+      <c r="B63" s="17">
+        <v>0.4375</v>
+      </c>
+      <c r="C63" s="17">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="D63" s="17">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E63" s="29"/>
+        <v>7.291666666666663E-2</v>
+      </c>
+      <c r="E63" s="29" t="s">
+        <v>104</v>
+      </c>
       <c r="F63" s="22"/>
       <c r="G63" s="18"/>
       <c r="H63" s="19"/>
     </row>
     <row r="64" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="3"/>
-      <c r="B64" s="4"/>
-      <c r="C64" s="4"/>
+      <c r="A64" s="3">
+        <v>44699</v>
+      </c>
+      <c r="B64" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C64" s="4">
+        <v>0.67083333333333339</v>
+      </c>
       <c r="D64" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E64" s="29"/>
-      <c r="F64" s="20"/>
+        <v>0.10833333333333339</v>
+      </c>
+      <c r="E64" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="F64" s="20" t="s">
+        <v>106</v>
+      </c>
       <c r="G64" s="6"/>
       <c r="H64" s="9"/>
     </row>
     <row r="65" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="30"/>
-      <c r="B65" s="17"/>
-      <c r="C65" s="17"/>
+      <c r="A65" s="30">
+        <v>44699</v>
+      </c>
+      <c r="B65" s="17">
+        <v>0.67083333333333339</v>
+      </c>
+      <c r="C65" s="17">
+        <v>0.70486111111111116</v>
+      </c>
       <c r="D65" s="17">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E65" s="29"/>
+        <v>3.4027777777777768E-2</v>
+      </c>
+      <c r="E65" s="29" t="s">
+        <v>107</v>
+      </c>
       <c r="F65" s="22"/>
       <c r="G65" s="18"/>
       <c r="H65" s="19"/>

</xml_diff>

<commit_message>
Mise a jour de la documentation concernant le pathfinding: il y a eu un rework par rapport aux documents précédents
</commit_message>
<xml_diff>
--- a/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
+++ b/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="116">
   <si>
     <t>Date</t>
   </si>
@@ -394,6 +394,34 @@
   </si>
   <si>
     <t>Documentation Datastructure/Architecture du programme</t>
+  </si>
+  <si>
+    <t>Changement de stratégie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'algorithme est très différent dans sont fonctionnement que les algorithme vu précédemment
+</t>
+  </si>
+  <si>
+    <t>Il faudra faire l'algorithme pas à pas ajoutant les complexité une a une afin de:
+1) etre plus efficace dans son implémnentation
+2) proposer une documentation plus structuré et améliorer la compréhension</t>
+  </si>
+  <si>
+    <t>HPA: Conception D'un chunk</t>
+  </si>
+  <si>
+    <t>But:
+Montrer la logique des emplacement des portes et les chemins qui les relient entre elle sans se préoccuper des partitions adjacentes pour le moment</t>
+  </si>
+  <si>
+    <t>Analyse et documentation des besoins pour l'algorithme</t>
+  </si>
+  <si>
+    <t>implémentations</t>
+  </si>
+  <si>
+    <t>Quelque soucis dans les container utilisé</t>
   </si>
 </sst>
 </file>
@@ -1378,8 +1406,8 @@
   </sheetPr>
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2840,54 +2868,94 @@
       <c r="H65" s="19"/>
     </row>
     <row r="66" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="3"/>
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
+      <c r="A66" s="3">
+        <v>44700</v>
+      </c>
+      <c r="B66" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C66" s="4">
+        <v>0.39305555555555555</v>
+      </c>
       <c r="D66" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E66" s="29"/>
-      <c r="F66" s="20"/>
-      <c r="G66" s="6"/>
+        <v>5.9722222222222232E-2</v>
+      </c>
+      <c r="E66" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="F66" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>110</v>
+      </c>
       <c r="H66" s="9"/>
     </row>
     <row r="67" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="30"/>
-      <c r="B67" s="17"/>
-      <c r="C67" s="17"/>
+      <c r="A67" s="30">
+        <v>44700</v>
+      </c>
+      <c r="B67" s="17">
+        <v>0.39305555555555555</v>
+      </c>
+      <c r="C67" s="17">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="D67" s="17">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E67" s="29"/>
-      <c r="F67" s="22"/>
+        <v>0.11736111111111108</v>
+      </c>
+      <c r="E67" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="F67" s="22" t="s">
+        <v>112</v>
+      </c>
       <c r="G67" s="18"/>
       <c r="H67" s="19"/>
     </row>
     <row r="68" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="3"/>
-      <c r="B68" s="4"/>
-      <c r="C68" s="4"/>
+      <c r="A68" s="3">
+        <v>44700</v>
+      </c>
+      <c r="B68" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C68" s="4">
+        <v>0.65416666666666667</v>
+      </c>
       <c r="D68" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E68" s="29"/>
+        <v>9.1666666666666674E-2</v>
+      </c>
+      <c r="E68" s="29" t="s">
+        <v>113</v>
+      </c>
       <c r="F68" s="20"/>
       <c r="G68" s="6"/>
       <c r="H68" s="9"/>
     </row>
     <row r="69" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="30"/>
-      <c r="B69" s="17"/>
-      <c r="C69" s="17"/>
+      <c r="A69" s="30">
+        <v>44700</v>
+      </c>
+      <c r="B69" s="17">
+        <v>0.65416666666666667</v>
+      </c>
+      <c r="C69" s="17">
+        <v>0.70486111111111116</v>
+      </c>
       <c r="D69" s="17">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E69" s="29"/>
-      <c r="F69" s="22"/>
+        <v>5.0694444444444486E-2</v>
+      </c>
+      <c r="E69" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="F69" s="22" t="s">
+        <v>115</v>
+      </c>
       <c r="G69" s="18"/>
       <c r="H69" s="19"/>
     </row>

</xml_diff>

<commit_message>
Remise en forme de la documentation: point final à la conception  + ajout des tests de validations + début réalisation
</commit_message>
<xml_diff>
--- a/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
+++ b/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="123">
   <si>
     <t>Date</t>
   </si>
@@ -422,6 +422,30 @@
   </si>
   <si>
     <t>Quelque soucis dans les container utilisé</t>
+  </si>
+  <si>
+    <t>Révision de la structure et orthographe, mise en page et partie manquante/remise à plus tard</t>
+  </si>
+  <si>
+    <t>Test par des tier</t>
+  </si>
+  <si>
+    <t>Mise en place de l'environnement + Build
+Testeurs:
+Antoine Dubois
+Gaetan Epars</t>
+  </si>
+  <si>
+    <t>Quelques tests sont mals formulés d'autres sont carrément faut dans le résultats attendu</t>
+  </si>
+  <si>
+    <t>Dossier de réalisation</t>
+  </si>
+  <si>
+    <t>Il faut lier le pathfinding avec le system de mouvement actuelle! Et faire un système de tir!</t>
+  </si>
+  <si>
+    <t>Partie régiment</t>
   </si>
 </sst>
 </file>
@@ -1406,8 +1430,8 @@
   </sheetPr>
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2960,66 +2984,116 @@
       <c r="H69" s="19"/>
     </row>
     <row r="70" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="3"/>
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
+      <c r="A70" s="3">
+        <v>44704</v>
+      </c>
+      <c r="B70" s="4">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="C70" s="4">
+        <v>0.48958333333333331</v>
+      </c>
       <c r="D70" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E70" s="29"/>
-      <c r="F70" s="20"/>
+        <v>7.9861111111111049E-2</v>
+      </c>
+      <c r="E70" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="F70" s="20" t="s">
+        <v>116</v>
+      </c>
       <c r="G70" s="6"/>
       <c r="H70" s="9"/>
     </row>
     <row r="71" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="30"/>
-      <c r="B71" s="17"/>
-      <c r="C71" s="17"/>
+      <c r="A71" s="30">
+        <v>44704</v>
+      </c>
+      <c r="B71" s="17">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="C71" s="17">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="D71" s="17">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E71" s="29"/>
-      <c r="F71" s="22"/>
-      <c r="G71" s="18"/>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="E71" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F71" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="G71" s="18" t="s">
+        <v>119</v>
+      </c>
       <c r="H71" s="19"/>
     </row>
     <row r="72" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="3"/>
-      <c r="B72" s="4"/>
-      <c r="C72" s="4"/>
+      <c r="A72" s="3">
+        <v>44704</v>
+      </c>
+      <c r="B72" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C72" s="4">
+        <v>0.57638888888888895</v>
+      </c>
       <c r="D72" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E72" s="29"/>
-      <c r="F72" s="20"/>
+        <v>1.3888888888888951E-2</v>
+      </c>
+      <c r="E72" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="F72" s="20" t="s">
+        <v>122</v>
+      </c>
       <c r="G72" s="6"/>
       <c r="H72" s="9"/>
     </row>
     <row r="73" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="30"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="17"/>
+      <c r="A73" s="30">
+        <v>44704</v>
+      </c>
+      <c r="B73" s="17">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="C73" s="17">
+        <v>0.59375</v>
+      </c>
       <c r="D73" s="17">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E73" s="29"/>
-      <c r="F73" s="22"/>
+        <v>1.7361111111111049E-2</v>
+      </c>
+      <c r="E73" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="F73" s="22" t="s">
+        <v>121</v>
+      </c>
       <c r="G73" s="18"/>
       <c r="H73" s="19"/>
     </row>
     <row r="74" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="3"/>
-      <c r="B74" s="4"/>
-      <c r="C74" s="4"/>
+      <c r="A74" s="3">
+        <v>44704</v>
+      </c>
+      <c r="B74" s="4">
+        <v>0.59375</v>
+      </c>
+      <c r="C74" s="4">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="D74" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E74" s="29"/>
+        <v>3.472222222222221E-2</v>
+      </c>
+      <c r="E74" s="29" t="s">
+        <v>120</v>
+      </c>
       <c r="F74" s="20"/>
       <c r="G74" s="6"/>
       <c r="H74" s="9"/>

</xml_diff>

<commit_message>
Correction de la fonctionnalité de tir + ajout pathfinding + Documentation, partie réalisation
</commit_message>
<xml_diff>
--- a/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
+++ b/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="127">
   <si>
     <t>Date</t>
   </si>
@@ -446,6 +446,18 @@
   </si>
   <si>
     <t>Partie régiment</t>
+  </si>
+  <si>
+    <t>implémentation système de tir</t>
+  </si>
+  <si>
+    <t>Implémentation du système de HPA au projet</t>
+  </si>
+  <si>
+    <t>Difficulté lié à la structure particulière des régiments</t>
+  </si>
+  <si>
+    <t>Documentation: Réalisation</t>
   </si>
 </sst>
 </file>
@@ -645,7 +657,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -735,6 +747,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1110,8 +1125,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Journal" displayName="Journal" ref="A1:H81" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8">
-  <autoFilter ref="A1:H81"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Journal" displayName="Journal" ref="A1:H87" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8">
+  <autoFilter ref="A1:H87"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Date" dataDxfId="7"/>
     <tableColumn id="2" name="Début" dataDxfId="6"/>
@@ -1428,10 +1443,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:H87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2384,7 +2399,7 @@
         <v>0.36805555555555558</v>
       </c>
       <c r="D42" s="4">
-        <f t="shared" ref="D42:D81" si="7">C42-B42</f>
+        <f t="shared" ref="D42:D87" si="7">C42-B42</f>
         <v>3.4722222222222265E-2</v>
       </c>
       <c r="E42" s="29" t="s">
@@ -3099,53 +3114,87 @@
       <c r="H74" s="9"/>
     </row>
     <row r="75" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="30"/>
-      <c r="B75" s="17"/>
-      <c r="C75" s="17"/>
+      <c r="A75" s="30">
+        <v>44705</v>
+      </c>
+      <c r="B75" s="17">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C75" s="17">
+        <v>0.37152777777777773</v>
+      </c>
       <c r="D75" s="17">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E75" s="29"/>
+        <v>3.819444444444442E-2</v>
+      </c>
+      <c r="E75" s="29" t="s">
+        <v>123</v>
+      </c>
       <c r="F75" s="22"/>
       <c r="G75" s="18"/>
       <c r="H75" s="19"/>
     </row>
     <row r="76" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="3"/>
-      <c r="B76" s="4"/>
-      <c r="C76" s="4"/>
+      <c r="A76" s="3">
+        <v>44705</v>
+      </c>
+      <c r="B76" s="4">
+        <v>0.37152777777777773</v>
+      </c>
+      <c r="C76" s="4">
+        <v>0.39930555555555558</v>
+      </c>
       <c r="D76" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E76" s="29"/>
-      <c r="F76" s="20"/>
+        <v>2.7777777777777846E-2</v>
+      </c>
+      <c r="E76" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="F76" s="20" t="s">
+        <v>125</v>
+      </c>
       <c r="G76" s="6"/>
       <c r="H76" s="9"/>
     </row>
     <row r="77" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="30"/>
-      <c r="B77" s="17"/>
-      <c r="C77" s="17"/>
+      <c r="A77" s="30">
+        <v>44705</v>
+      </c>
+      <c r="B77" s="17">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="C77" s="17">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="D77" s="17">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E77" s="29"/>
+        <v>0.11111111111111105</v>
+      </c>
+      <c r="E77" s="29" t="s">
+        <v>126</v>
+      </c>
       <c r="F77" s="22"/>
       <c r="G77" s="18"/>
       <c r="H77" s="19"/>
     </row>
     <row r="78" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="3"/>
-      <c r="B78" s="4"/>
-      <c r="C78" s="4"/>
+      <c r="A78" s="3">
+        <v>44705</v>
+      </c>
+      <c r="B78" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C78" s="4">
+        <v>0.67013888888888884</v>
+      </c>
       <c r="D78" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E78" s="29"/>
+        <v>0.10763888888888884</v>
+      </c>
+      <c r="E78" s="29" t="s">
+        <v>25</v>
+      </c>
       <c r="F78" s="20"/>
       <c r="G78" s="6"/>
       <c r="H78" s="9"/>
@@ -3164,50 +3213,128 @@
       <c r="H79" s="19"/>
     </row>
     <row r="80" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="3">
+      <c r="A80" s="31"/>
+      <c r="B80" s="23"/>
+      <c r="C80" s="23"/>
+      <c r="D80" s="23">
+        <f t="shared" ref="D80:D81" si="8">C80-B80</f>
+        <v>0</v>
+      </c>
+      <c r="E80" s="29"/>
+      <c r="F80" s="24"/>
+      <c r="G80" s="25"/>
+      <c r="H80" s="9"/>
+    </row>
+    <row r="81" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="31"/>
+      <c r="B81" s="23"/>
+      <c r="C81" s="23"/>
+      <c r="D81" s="23">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E81" s="29"/>
+      <c r="F81" s="24"/>
+      <c r="G81" s="25"/>
+      <c r="H81" s="9"/>
+    </row>
+    <row r="82" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="31"/>
+      <c r="B82" s="23"/>
+      <c r="C82" s="23"/>
+      <c r="D82" s="23">
+        <f t="shared" ref="D82:D83" si="9">C82-B82</f>
+        <v>0</v>
+      </c>
+      <c r="E82" s="29"/>
+      <c r="F82" s="24"/>
+      <c r="G82" s="25"/>
+      <c r="H82" s="9"/>
+    </row>
+    <row r="83" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="31"/>
+      <c r="B83" s="23"/>
+      <c r="C83" s="23"/>
+      <c r="D83" s="23">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="E83" s="29"/>
+      <c r="F83" s="24"/>
+      <c r="G83" s="25"/>
+      <c r="H83" s="9"/>
+    </row>
+    <row r="84" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="31"/>
+      <c r="B84" s="23"/>
+      <c r="C84" s="23"/>
+      <c r="D84" s="23">
+        <f t="shared" ref="D84:D85" si="10">C84-B84</f>
+        <v>0</v>
+      </c>
+      <c r="E84" s="29"/>
+      <c r="F84" s="24"/>
+      <c r="G84" s="25"/>
+      <c r="H84" s="9"/>
+    </row>
+    <row r="85" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="31"/>
+      <c r="B85" s="23"/>
+      <c r="C85" s="23"/>
+      <c r="D85" s="23">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E85" s="29"/>
+      <c r="F85" s="24"/>
+      <c r="G85" s="25"/>
+      <c r="H85" s="9"/>
+    </row>
+    <row r="86" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3">
         <v>44659</v>
       </c>
-      <c r="B80" s="4">
+      <c r="B86" s="4">
         <v>12.020833333333499</v>
       </c>
-      <c r="C80" s="4">
+      <c r="C86" s="4">
         <v>12.086805555555699</v>
       </c>
-      <c r="D80" s="4">
+      <c r="D86" s="4">
         <f t="shared" si="7"/>
         <v>6.5972222222200116E-2</v>
       </c>
-      <c r="E80" s="29" t="s">
+      <c r="E86" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="F80" s="20" t="s">
+      <c r="F86" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G80" s="6"/>
-      <c r="H80" s="9"/>
-    </row>
-    <row r="81" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="30">
+      <c r="G86" s="6"/>
+      <c r="H86" s="9"/>
+    </row>
+    <row r="87" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="30">
         <v>44660</v>
       </c>
-      <c r="B81" s="17">
+      <c r="B87" s="17">
         <v>12.250000000000099</v>
       </c>
-      <c r="C81" s="17">
+      <c r="C87" s="17">
         <v>12.3159722222223</v>
       </c>
-      <c r="D81" s="17">
+      <c r="D87" s="17">
         <f t="shared" si="7"/>
         <v>6.5972222222200116E-2</v>
       </c>
-      <c r="E81" s="29" t="s">
+      <c r="E87" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="F81" s="22" t="s">
+      <c r="F87" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="G81" s="18"/>
-      <c r="H81" s="19"/>
+      <c r="G87" s="18"/>
+      <c r="H87" s="19"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Finalisation de la documentation: Conclusion, réalisation, résumé
</commit_message>
<xml_diff>
--- a/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
+++ b/Assets/Documentation/FlorianDuruz_JournalDeTravail_CastleDefense.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="132">
   <si>
     <t>Date</t>
   </si>
@@ -458,6 +458,23 @@
   </si>
   <si>
     <t>Documentation: Réalisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documentation: Stratégie de test + Réalisation </t>
+  </si>
+  <si>
+    <t>Scéance Tests</t>
+  </si>
+  <si>
+    <t>Testeurs:
+Azad Saffai
+Thirusan Rajadurai</t>
+  </si>
+  <si>
+    <t>Documentation Fin réalisation + tests effectué</t>
+  </si>
+  <si>
+    <t>Documentation: Conclusion + résumé</t>
   </si>
 </sst>
 </file>
@@ -1445,8 +1462,8 @@
   </sheetPr>
   <dimension ref="A1:H87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="F80" sqref="F80"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3200,53 +3217,87 @@
       <c r="H78" s="9"/>
     </row>
     <row r="79" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="30"/>
-      <c r="B79" s="17"/>
-      <c r="C79" s="17"/>
+      <c r="A79" s="30">
+        <v>44706</v>
+      </c>
+      <c r="B79" s="17">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="C79" s="17">
+        <v>0.39583333333333331</v>
+      </c>
       <c r="D79" s="17">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E79" s="29"/>
+        <v>2.7777777777777735E-2</v>
+      </c>
+      <c r="E79" s="29" t="s">
+        <v>127</v>
+      </c>
       <c r="F79" s="22"/>
       <c r="G79" s="18"/>
       <c r="H79" s="19"/>
     </row>
     <row r="80" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="31"/>
-      <c r="B80" s="23"/>
-      <c r="C80" s="23"/>
+      <c r="A80" s="26">
+        <v>44706</v>
+      </c>
+      <c r="B80" s="23">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="C80" s="23">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="D80" s="23">
         <f t="shared" ref="D80:D81" si="8">C80-B80</f>
-        <v>0</v>
-      </c>
-      <c r="E80" s="29"/>
-      <c r="F80" s="24"/>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="E80" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="F80" s="24" t="s">
+        <v>129</v>
+      </c>
       <c r="G80" s="25"/>
       <c r="H80" s="9"/>
     </row>
     <row r="81" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="31"/>
-      <c r="B81" s="23"/>
-      <c r="C81" s="23"/>
+      <c r="A81" s="26">
+        <v>44706</v>
+      </c>
+      <c r="B81" s="23">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C81" s="23">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="D81" s="23">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="E81" s="29"/>
+        <v>9.3749999999999944E-2</v>
+      </c>
+      <c r="E81" s="29" t="s">
+        <v>130</v>
+      </c>
       <c r="F81" s="24"/>
       <c r="G81" s="25"/>
       <c r="H81" s="9"/>
     </row>
     <row r="82" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="31"/>
-      <c r="B82" s="23"/>
-      <c r="C82" s="23"/>
+      <c r="A82" s="26">
+        <v>44706</v>
+      </c>
+      <c r="B82" s="23">
+        <v>0.5625</v>
+      </c>
+      <c r="C82" s="23">
+        <v>0.70486111111111116</v>
+      </c>
       <c r="D82" s="23">
         <f t="shared" ref="D82:D83" si="9">C82-B82</f>
-        <v>0</v>
-      </c>
-      <c r="E82" s="29"/>
+        <v>0.14236111111111116</v>
+      </c>
+      <c r="E82" s="29" t="s">
+        <v>131</v>
+      </c>
       <c r="F82" s="24"/>
       <c r="G82" s="25"/>
       <c r="H82" s="9"/>

</xml_diff>